<commit_message>
Adding curve fitting to the AD notebook.
Curve fitting using the Gompertz equation was added to the notebook to
simulate methane production potential from the acetate experiments.
</commit_message>
<xml_diff>
--- a/spreadsheets/bmp_acetate_test_kinetics.xlsx
+++ b/spreadsheets/bmp_acetate_test_kinetics.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Acet_Test_4" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="Acet_Test_Ac" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="No_Feed_Ac" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Kinetic_Data" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="69">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -202,6 +203,36 @@
   </si>
   <si>
     <t xml:space="preserve">27/03_19:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane Production Potential (ml CH4/g sCOD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane Production Rate (ml CH4/g sCOD min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lag Time (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_squared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Ac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample 4</t>
   </si>
 </sst>
 </file>
@@ -217,6 +248,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -276,12 +308,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,6 +331,485 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>583920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>27000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>200520</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5732640" y="352080"/>
+          <a:ext cx="6931800" cy="4493880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>711360</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>53640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>325440</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6100560" y="216360"/>
+          <a:ext cx="6929280" cy="4493880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>747000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>361080</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>32400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6136200" y="252720"/>
+          <a:ext cx="6929280" cy="4493880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>598320</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>126720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>212400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>69120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 9" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987520" y="289440"/>
+          <a:ext cx="6929280" cy="4493880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>122040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>549000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>105120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 10" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324120" y="325440"/>
+          <a:ext cx="6929280" cy="4493880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>500040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>72360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>713880</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>122760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 11" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5889240" y="72360"/>
+          <a:ext cx="5090760" cy="3301560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>669240</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>23760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 12" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5871600" y="3567240"/>
+          <a:ext cx="5063760" cy="3283920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>382320</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>45360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1501200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>18360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="382320" y="1183320"/>
+          <a:ext cx="4961160" cy="3224160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1655280</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>354240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5497560" y="1153080"/>
+          <a:ext cx="5006520" cy="3253680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1295640</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>112320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266400" y="4749480"/>
+          <a:ext cx="4871520" cy="3165840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1846800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>301320</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>59400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5689080" y="4767480"/>
+          <a:ext cx="4762080" cy="3094920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>534240</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>126360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>696240</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>150120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10684080" y="2239560"/>
+          <a:ext cx="5038920" cy="3274920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,330 +931,330 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>13.967</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>0.232783333333333</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>73.986</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>1.2331</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>133.981</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>2.23301666666667</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>23.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>193.993</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>3.23321666666667</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>230.339</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>3.83898333333333</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>30.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>290.327</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>4.83878333333333</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>350.322</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>5.8387</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>363.719</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>6.06198333333333</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>37.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>423.727</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>7.06211666666667</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>39.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>483.722</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>8.06203333333333</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>41.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>509.669</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <v>8.49448333333333</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>42.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>569.668</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>9.49446666666667</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>43.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>629.657</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="2" t="n">
         <v>10.4942833333333</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>44.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>689.661</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="2" t="n">
         <v>11.49435</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>45.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>749.66</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="2" t="n">
         <v>12.4943333333333</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>46.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>809.683</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <v>13.4947166666667</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>869.926</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="2" t="n">
         <v>14.4987666666667</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>47.5</v>
       </c>
     </row>
@@ -751,6 +1266,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -767,228 +1283,228 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>61.304</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>1.02173333333333</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>181.303</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>3.02171666666667</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>301.313</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>5.02188333333333</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>421.307</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>7.02178333333333</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>21.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>541.305</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>9.02175</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>661.31</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>11.0218333333333</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>781.308</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>13.0218</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>25.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>901.313</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>15.0218833333333</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>26.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>1021.322</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>17.0220333333333</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1141.316</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>19.0219333333333</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>27.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>1261.325</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <v>21.0220833333333</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>28</v>
       </c>
     </row>
@@ -1000,6 +1516,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1016,262 +1533,262 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>25.947</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>0.43245</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>85.946</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>1.43243333333333</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>145.935</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>2.43225</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>5.5</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>16.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>205.939</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>3.43231666666667</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>265.938</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>4.4323</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>23.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>325.961</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>5.43268333333333</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>25.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>386.204</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>6.43673333333333</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>26.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>427.148</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>7.11913333333333</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>27.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>487.142</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>8.11903333333333</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>28.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>547.153</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>9.11921666666667</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>607.15</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <v>10.1191666666667</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>29.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>667.16</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>11.1193333333333</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>0.45</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>29.95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>722.272</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="2" t="n">
         <v>12.0378666666667</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>30</v>
       </c>
     </row>
@@ -1283,6 +1800,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1294,199 +1812,199 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>13.397</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>0.223283333333333</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>73.405</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>1.22341666666667</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>133.4</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>2.22333333333333</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>159.347</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>2.65578333333333</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>219.346</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>3.65576666666667</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>279.335</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>4.65558333333333</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>339.339</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>5.65565</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>399.338</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>6.65563333333333</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>459.361</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>7.65601666666667</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>47</v>
       </c>
     </row>
@@ -1498,6 +2016,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1509,352 +2028,352 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>36.346</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>0.605766666666667</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>6.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>96.334</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>1.60556666666667</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>11.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>156.329</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>2.60548333333333</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>14.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>169.726</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>2.82876666666667</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>229.734</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>3.8289</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>16.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>289.729</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>4.82881666666667</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>315.676</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>5.26126666666667</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>18.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>375.675</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>6.26125</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>19.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>435.664</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>7.26106666666667</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>495.668</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>8.26113333333333</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>20.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>555.667</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <v>9.26111666666667</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>20.8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>615.69</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>10.2615</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>675.933</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="2" t="n">
         <v>11.26555</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>21.2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>716.877</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="2" t="n">
         <v>11.94795</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>21.3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>776.871</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="2" t="n">
         <v>12.94785</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>21.35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>836.882</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <v>13.9480333333333</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>21.4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>896.879</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="2" t="n">
         <v>14.9479833333333</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>21.45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>956.889</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="2" t="n">
         <v>15.94815</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -1866,6 +2385,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1877,607 +2397,607 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>61.304</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>1.02173333333333</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>181.303</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>3.02171666666667</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>301.313</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>5.02188333333333</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>421.307</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>7.02178333333333</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>541.305</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>9.02175</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>661.31</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>11.0218333333333</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>781.308</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>13.0218</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>25.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>901.313</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>15.0218833333333</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>1021.322</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>17.0220333333333</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>30.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1141.316</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>19.0219333333333</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>1261.325</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <v>21.0220833333333</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>1381.328</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>23.0221333333333</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>1501.327</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="2" t="n">
         <v>25.0221166666667</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>1621.332</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="2" t="n">
         <v>27.0222</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>38.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>1741.33</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="2" t="n">
         <v>29.0221666666667</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>1750.422</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <v>29.1737</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>39.1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="n">
+      <c r="B21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>120.003</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="2" t="n">
         <v>2.00005</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>240.012</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="C23" s="2" t="n">
         <v>4.0002</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>360.017</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="C24" s="2" t="n">
         <v>6.00028333333333</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>480.028</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="2" t="n">
         <v>8.00046666666667</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>600.03</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="2" t="n">
         <v>10.0005</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>720.028</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="2" t="n">
         <v>12.0004666666667</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>840.024</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C28" s="2" t="n">
         <v>14.0004</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>960.032</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="2" t="n">
         <v>16.0005333333333</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>1080.026</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="2" t="n">
         <v>18.0004333333333</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>1200.024</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="2" t="n">
         <v>20.0004</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>23.5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>1320.034</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="C32" s="2" t="n">
         <v>22.0005666666667</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>1440.026</v>
       </c>
-      <c r="C33" s="1" t="n">
+      <c r="C33" s="2" t="n">
         <v>24.0004333333333</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>1560.025</v>
       </c>
-      <c r="C34" s="1" t="n">
+      <c r="C34" s="2" t="n">
         <v>26.0004166666667</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>30.5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>1680.031</v>
       </c>
-      <c r="C35" s="1" t="n">
+      <c r="C35" s="2" t="n">
         <v>28.0005166666667</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>1784.318</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="2" t="n">
         <v>29.7386333333333</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>35</v>
       </c>
     </row>
@@ -2489,5 +3009,139 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.79"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>210.502175331624</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>44.6513434110361</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.918532257427795</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>452.518550919028</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>80.3875654506543</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.96980778921661</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>259.039403662575</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>45.9301994884574</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.885690609598239</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>292.865347431964</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>61.9142657259945</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.988846242898073</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>466.304417599042</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>97.7190568550102</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.989664759854468</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>